<commit_message>
Added stuff for phase 2
Former-commit-id: 10da94e102e25f437e557f08706e5069448406a3
</commit_message>
<xml_diff>
--- a/Credit_Risk_credit_assignment.xlsx
+++ b/Credit_Risk_credit_assignment.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IndianaU\CSCI-P556-AML\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F85B1F-4F38-4621-8DF0-6A1BE5FEBAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37899D9E-7AE6-49AB-AEEB-82582FCDFE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="1596" windowWidth="18816" windowHeight="8712" xr2:uid="{82E302A5-59BB-48C1-9A38-E30F714E3CFB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{82E302A5-59BB-48C1-9A38-E30F714E3CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Phase 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">'Phase 1'!$A1048576</definedName>
+    <definedName name="prevWBS" localSheetId="1">'Phase 2'!$A1048576</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Home Credit Default Risk</t>
   </si>
@@ -75,13 +77,46 @@
   </si>
   <si>
     <t>Glen Collecti</t>
+  </si>
+  <si>
+    <t>Phase 2: EDA and baseline pipeline. Team Lead: Paul Miller</t>
+  </si>
+  <si>
+    <t>Load data</t>
+  </si>
+  <si>
+    <t>Record video</t>
+  </si>
+  <si>
+    <t>All members</t>
+  </si>
+  <si>
+    <t>Credit Assignment</t>
+  </si>
+  <si>
+    <t>Create presentation slides</t>
+  </si>
+  <si>
+    <t>Baseline models and pipelines. XGBoost, KNN, Logistic Regression</t>
+  </si>
+  <si>
+    <t>Abstract, organize notebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDA </t>
+  </si>
+  <si>
+    <t>Visual EDA</t>
+  </si>
+  <si>
+    <t>Glen Colletti</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +218,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -217,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -245,11 +285,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -298,11 +349,43 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -661,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE0CAC1-6873-4028-950B-4EEAE5783709}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,7 +849,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="str">
-        <f t="shared" ref="A5:A9" si="0">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A5:A8" si="0">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -878,15 +961,262 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4:R8">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>#REF!=TODAY()</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4:R8">
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>AND(#REF!&lt;=#REF!,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=#REF!)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
+      <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD04EF87-9E51-433D-ACFB-B2689D00B139}">
+  <dimension ref="A1:R12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="53.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D4:R8">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>#REF!=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND(#REF!&lt;=#REF!,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=#REF!)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated credit assignment file
Former-commit-id: f194e57f68e371b30a5d0a9028a2c806c2f96d9b
</commit_message>
<xml_diff>
--- a/Credit_Risk_credit_assignment.xlsx
+++ b/Credit_Risk_credit_assignment.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IndianaU\CSCI-P556-AML\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F85B1F-4F38-4621-8DF0-6A1BE5FEBAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37899D9E-7AE6-49AB-AEEB-82582FCDFE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="1596" windowWidth="18816" windowHeight="8712" xr2:uid="{82E302A5-59BB-48C1-9A38-E30F714E3CFB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{82E302A5-59BB-48C1-9A38-E30F714E3CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Phase 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Phase 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">'Phase 1'!$A1048576</definedName>
+    <definedName name="prevWBS" localSheetId="1">'Phase 2'!$A1048576</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Home Credit Default Risk</t>
   </si>
@@ -75,13 +77,46 @@
   </si>
   <si>
     <t>Glen Collecti</t>
+  </si>
+  <si>
+    <t>Phase 2: EDA and baseline pipeline. Team Lead: Paul Miller</t>
+  </si>
+  <si>
+    <t>Load data</t>
+  </si>
+  <si>
+    <t>Record video</t>
+  </si>
+  <si>
+    <t>All members</t>
+  </si>
+  <si>
+    <t>Credit Assignment</t>
+  </si>
+  <si>
+    <t>Create presentation slides</t>
+  </si>
+  <si>
+    <t>Baseline models and pipelines. XGBoost, KNN, Logistic Regression</t>
+  </si>
+  <si>
+    <t>Abstract, organize notebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDA </t>
+  </si>
+  <si>
+    <t>Visual EDA</t>
+  </si>
+  <si>
+    <t>Glen Colletti</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +218,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -217,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -245,11 +285,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -298,11 +349,43 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -661,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE0CAC1-6873-4028-950B-4EEAE5783709}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,7 +849,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="str">
-        <f t="shared" ref="A5:A9" si="0">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A5:A8" si="0">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -878,15 +961,262 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4:R8">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>#REF!=TODAY()</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4:R8">
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>AND(#REF!&lt;=#REF!,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=#REF!)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
+      <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD04EF87-9E51-433D-ACFB-B2689D00B139}">
+  <dimension ref="A1:R12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="53.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D4:R8">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>#REF!=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND(#REF!&lt;=#REF!,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=#REF!)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=#REF!,#REF!&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>